<commit_message>
commit after adding testSummary
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Script.xlsx
+++ b/src/test/resources/Test_Script.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408719\IdeaProjects\CarWashServices\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD3FC435-69D9-48DE-A58B-3D2C400D8CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76253D57-5B02-4A2A-A42B-73EF9AA4BABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{57A7AD9C-5043-4A2A-A59C-DE6B97F2DC06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Test Script ID</t>
   </si>
@@ -86,9 +86,6 @@
     <t>1. Open the Justdail website</t>
   </si>
   <si>
-    <t>1. pecify the Location as detected location</t>
-  </si>
-  <si>
     <t>2. search for CarWashServices</t>
   </si>
   <si>
@@ -147,6 +144,20 @@
   </si>
   <si>
     <t>Zym items are retrieved successfully</t>
+  </si>
+  <si>
+    <t>1. Specify the Location as detected location</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>SearchKey: Car Washing Services
+Rating: 4
+Number of services to show:5</t>
+  </si>
+  <si>
+    <t>Phone Number: 123</t>
   </si>
 </sst>
 </file>
@@ -214,19 +225,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -566,7 +580,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+      <selection activeCell="H2" sqref="H2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,10 +590,10 @@
     <col min="3" max="3" width="19.08984375" customWidth="1"/>
     <col min="4" max="4" width="15.6328125" customWidth="1"/>
     <col min="5" max="5" width="24.26953125" customWidth="1"/>
-    <col min="6" max="6" width="24.453125" customWidth="1"/>
+    <col min="6" max="6" width="42.36328125" customWidth="1"/>
     <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.7265625" customWidth="1"/>
-    <col min="9" max="9" width="19.453125" customWidth="1"/>
+    <col min="8" max="8" width="42.36328125" customWidth="1"/>
+    <col min="9" max="9" width="41.26953125" customWidth="1"/>
     <col min="10" max="10" width="17.54296875" customWidth="1"/>
     <col min="11" max="11" width="20.6328125" customWidth="1"/>
   </cols>
@@ -622,181 +636,175 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:12" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:12" ht="26" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="38.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="E5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" spans="1:12" ht="26" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" ht="26" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="E7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" ht="26" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="J2:J4"/>
@@ -813,6 +821,22 @@
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>